<commit_message>
prepare OCP and SDP for dist to Sion
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellSionGuess-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellSionGuess-P2DM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60867F8F-BCC9-49CA-9706-9BA2862926EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558B6488-5738-4D48-AA1A-D6DD4C54D8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="21570" windowHeight="12870" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="16" r:id="rId1"/>
@@ -1656,45 +1656,45 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="491">
@@ -2574,8 +2574,8 @@
   </sheetPr>
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2613,33 +2613,33 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="36" hidden="1" customHeight="1">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="46"/>
     </row>
     <row r="3" spans="1:7" ht="16.5" thickBot="1">
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:7" ht="12" customHeight="1" thickBot="1"/>
     <row r="5" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="43"/>
     </row>
     <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="32" t="s">
@@ -2711,14 +2711,14 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="32" t="s">
@@ -2773,7 +2773,7 @@
       <c r="D13" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="40">
         <v>1E-8</v>
       </c>
       <c r="F13" s="22">
@@ -2790,14 +2790,14 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="43"/>
     </row>
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="32" t="s">
@@ -2970,14 +2970,14 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="43"/>
     </row>
     <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="32" t="s">
@@ -3173,7 +3173,7 @@
         <v>163</v>
       </c>
       <c r="E35" s="33">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F35" s="22">
         <v>0</v>
@@ -3189,14 +3189,14 @@
       <c r="G36" s="20"/>
     </row>
     <row r="37" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A38" t="s">
@@ -3288,14 +3288,14 @@
       <c r="G42" s="20"/>
     </row>
     <row r="43" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="42"/>
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
+      <c r="G43" s="43"/>
     </row>
     <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="32" t="s">
@@ -3386,14 +3386,14 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="32.1" customHeight="1" thickBot="1">
-      <c r="B49" s="40" t="s">
+      <c r="B49" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="F49" s="42"/>
+      <c r="G49" s="43"/>
     </row>
     <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="32" t="s">
@@ -3809,7 +3809,7 @@
         <v>163</v>
       </c>
       <c r="E70" s="33">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F70" s="22">
         <v>0</v>

</xml_diff>

<commit_message>
Interchangeable solid diffusion and kinetics models for linear eis regression
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellSionGuess-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellSionGuess-P2DM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180923A1-D88F-4BEB-815A-2BDDA73F92DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9327F38E-36D1-42A3-B0C8-D21D0612BE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="21570" windowHeight="12870" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="201">
   <si>
     <t>Code Name</t>
   </si>
@@ -690,6 +690,27 @@
   </si>
   <si>
     <t>#pkg[Package]</t>
+  </si>
+  <si>
+    <t>Solid-phase diffusivity CPE-integrator time const.</t>
+  </si>
+  <si>
+    <t>tauF</t>
+  </si>
+  <si>
+    <t>\tau_\mathrm{f}</t>
+  </si>
+  <si>
+    <t>1/s</t>
+  </si>
+  <si>
+    <t>Empirical multiplicity of solid diffusivity</t>
+  </si>
+  <si>
+    <t>mD</t>
+  </si>
+  <si>
+    <t>m_\mathrm{D}</t>
   </si>
 </sst>
 </file>
@@ -2572,10 +2593,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3660,206 +3681,244 @@
     </row>
     <row r="63" spans="1:7" ht="15.95" customHeight="1">
       <c r="B63" s="6" t="s">
-        <v>15</v>
+        <v>198</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>68</v>
+        <v>199</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E63" s="22">
+        <v>200</v>
+      </c>
+      <c r="E63" s="37">
         <v>1</v>
       </c>
-      <c r="F63" s="22">
-        <v>0</v>
-      </c>
+      <c r="F63" s="22"/>
       <c r="G63" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="15.95" customHeight="1">
       <c r="B64" s="6" t="s">
-        <v>140</v>
+        <v>15</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="E64" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="F64" s="39">
+        <v>177</v>
+      </c>
+      <c r="E64" s="22">
+        <v>1</v>
+      </c>
+      <c r="F64" s="22">
         <v>0</v>
       </c>
       <c r="G64" s="8" t="s">
-        <v>142</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="15.95" customHeight="1">
       <c r="B65" s="6" t="s">
-        <v>141</v>
+        <v>194</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="E65" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="F65" s="39">
+        <v>196</v>
+      </c>
+      <c r="E65" s="22">
+        <v>100</v>
+      </c>
+      <c r="F65" s="22">
         <v>0</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>14</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="15.95" customHeight="1">
       <c r="B66" s="6" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E66" s="9">
-        <v>0.02</v>
-      </c>
-      <c r="F66" s="22">
+        <v>154</v>
+      </c>
+      <c r="E66" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="F66" s="39">
         <v>0</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="15.95" customHeight="1">
       <c r="B67" s="6" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E67" s="22">
-        <v>0.22</v>
-      </c>
-      <c r="F67" s="22">
+        <v>157</v>
+      </c>
+      <c r="E67" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="F67" s="39">
         <v>0</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="15.95" customHeight="1">
       <c r="B68" s="6" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E68" s="22">
-        <v>1</v>
+        <v>159</v>
+      </c>
+      <c r="E68" s="9">
+        <v>0.02</v>
       </c>
       <c r="F68" s="22">
         <v>0</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="15.95" customHeight="1">
       <c r="B69" s="6" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E69" s="22">
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="F69" s="22">
         <v>0</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="15.95" customHeight="1">
       <c r="B70" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E70" s="33">
-        <v>0.1</v>
+        <v>161</v>
+      </c>
+      <c r="E70" s="22">
+        <v>1</v>
       </c>
       <c r="F70" s="22">
         <v>0</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15.95" customHeight="1">
       <c r="B71" s="6" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E71" s="22">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F71" s="22">
         <v>0</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.95" customHeight="1">
       <c r="B72" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E72" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="F72" s="22">
+        <v>0</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B73" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E73" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="F73" s="22">
+        <v>0</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15.95" customHeight="1">
+      <c r="B74" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C74" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D72" s="6" t="s">
+      <c r="D74" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="E72" s="22">
+      <c r="E74" s="22">
         <v>1.5</v>
       </c>
-      <c r="F72" s="22">
-        <v>0</v>
-      </c>
-      <c r="G72" s="8" t="s">
+      <c r="F74" s="22">
+        <v>0</v>
+      </c>
+      <c r="G74" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
linear EIS regression stable
</commit_message>
<xml_diff>
--- a/GEN2_XLSX_CELLDEFS/cellSionGuess-P2DM.xlsx
+++ b/GEN2_XLSX_CELLDEFS/cellSionGuess-P2DM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CLiMB\LMB_Toolkit\GEN2_XLSX_CELLDEFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9327F38E-36D1-42A3-B0C8-D21D0612BE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F97C3A-D801-4572-BD08-22BA23E7D98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="15" windowWidth="21570" windowHeight="12870" tabRatio="629" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2596,7 +2596,7 @@
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3692,7 +3692,9 @@
       <c r="E63" s="37">
         <v>1</v>
       </c>
-      <c r="F63" s="22"/>
+      <c r="F63" s="22">
+        <v>0</v>
+      </c>
       <c r="G63" s="8" t="s">
         <v>14</v>
       </c>

</xml_diff>